<commit_message>
updated description of operations
</commit_message>
<xml_diff>
--- a/docs/excel tamplate QRA.xlsx
+++ b/docs/excel tamplate QRA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\BMR_Generator-1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4783C80-2FF1-454D-A18F-73B1D5029642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B703D69-0334-4A0F-BDF9-068E21459951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F9EF1FD-EDCF-417A-A688-B5B990E0C384}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Equipment:</t>
   </si>
@@ -46,9 +46,6 @@
     <t>druck filter</t>
   </si>
   <si>
-    <t>nutsch filter</t>
-  </si>
-  <si>
     <t>membrane pump</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>loading on filter</t>
   </si>
   <si>
-    <t>argon pressure</t>
-  </si>
-  <si>
     <t>discharging ML</t>
   </si>
   <si>
@@ -118,12 +112,6 @@
     <t>atm. distillation</t>
   </si>
   <si>
-    <t>Material is loaded into reactor via &lt;60 mm flange port&gt; using funnel &lt;funnel label&gt;</t>
-  </si>
-  <si>
-    <t>The &lt;60 mm flange port&gt; is closed.</t>
-  </si>
-  <si>
     <t>operation type:</t>
   </si>
   <si>
@@ -139,16 +127,99 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Required amount of the &lt;liquid material&gt; is weighed on the balance &lt;balance number&gt; using jug &lt;jub label&gt;.</t>
-  </si>
-  <si>
-    <t>Required amount of the &lt;solid material&gt; is weighed on the balance &lt;balance number&gt; using jug &lt;jug label&gt;.</t>
-  </si>
-  <si>
     <t>dosing liquid</t>
   </si>
   <si>
-    <t xml:space="preserve">Using peristaltic pump &lt;peristaltic pump number&gt; and norprene hose &lt;hose label&gt; &lt;liquid material&gt; is pumped into reactor via &lt;liquid loading valve&gt;. Peristaltic pump setting </t>
+    <t>Required amount of {material} is weighed on the {equipment: balances} using {utensils: jug}.
+Material is loaded into reactor via 60 mm flange port using {utensils: funnel}
+The 60 mm flange port is closed.</t>
+  </si>
+  <si>
+    <t>Product is loaded on the filter via product line. Argon line is closed during loading. Once 2/3 of the filter is loaded, stop pumping and close product line.</t>
+  </si>
+  <si>
+    <t>filtration with argon pressure</t>
+  </si>
+  <si>
+    <t>The lid of the filter is opened. Material from the filter is unloaded using {utensils: shovel} &lt;to where&gt;.</t>
+  </si>
+  <si>
+    <t>Nutsche filter</t>
+  </si>
+  <si>
+    <t>Stirring in reactor is turned OFF.</t>
+  </si>
+  <si>
+    <t>Heating is turned OFF.</t>
+  </si>
+  <si>
+    <t>Reactor is set up for vacuum distillation, all inlet connections are closed. Tap water to the condenser is connected and opened. Receiver is properly connected to the condenser.</t>
+  </si>
+  <si>
+    <t>The filter is assembled and prepared to work. Filtration cloth is prepared and properly installed. Argon and product lines are connected to the lid, pressure test is done.</t>
+  </si>
+  <si>
+    <t>Check that product line is closed, check the pressure on Argon cylinder, it must be in range 1-2bar. Open argon line on the lid of the filter and wait until no more or very little of ML is coming into the receiver (visually on level tube). At the end of operation close the argon line.</t>
+  </si>
+  <si>
+    <t>Membrane pump is started. Product is loaded on the filter using {utensils: jug}. Once 2/3 of the filter is loaded, stop loading.</t>
+  </si>
+  <si>
+    <t>The filter is assembled and prepared to work. Filtration cloth is prepared and properly installed.  {equipment: membrane pump} is connected.</t>
+  </si>
+  <si>
+    <t>The lid of filter is opened. Required amount of {material} is weighed on the {equipment: balances} using {utensils: jug}. Solvent isloaded on top of  filter caje, using shovel {utensils: shovel} the filter cake is thoroughly mixed. The lid is closed.</t>
+  </si>
+  <si>
+    <t>Make sure the pupm is stopped. Required amount of {material} is weighed on the {equipment: balances} using {utensils: jug}. Solvent is loaded on top of  filter caje, using shovel {utensils: shovel} the filter cake is thoroughly mixed.</t>
+  </si>
+  <si>
+    <t>{equipment: membrane pump} is set to {setting} Torrs.</t>
+  </si>
+  <si>
+    <t>{equipment: membrane pump} is set to {setting} %.</t>
+  </si>
+  <si>
+    <t>Required amount of {material} is weighed on the {equipment: balances} using {utensils: jug}. 
+Using peristaltic pump  {equipment: peristaltic pump} and {utensils: norprene hose}, {material} is pumped into reactor via liquid loading valve. Peristaltic pump is set to {setting}%.</t>
+  </si>
+  <si>
+    <t>Required amount of {material} is weighed on the {equipment: balances} using {utensils: jug}. 
+Using peristaltic pump  {equipment: peristaltic pump} and {utensils: norprene hose}, {material} is pumped into dosing system. Peristaltic pump is set to {setting}%.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon line is connected to the argon port of reactor. The flow is set to {setting}l/min. The valve is opened. </t>
+  </si>
+  <si>
+    <t>Stirring in reactor is turned ON. Set to {setting}rpm.</t>
+  </si>
+  <si>
+    <t>Heating is turned ON. Set to {setting}°C.</t>
+  </si>
+  <si>
+    <t>Cooling is turned ON. Set to {setting}°C.</t>
+  </si>
+  <si>
+    <t>Cooling is turned OFF.</t>
+  </si>
+  <si>
+    <t>Reactor is set up for vacuum distillation, all inlet connections are closed. Tap water to the condenser is connected and opened. Receiver is properly connected to the condenser.
+The membrane pump {equipment: membrane pump} is connected via cold trap, vacuum is set {setting}Torr. Cold trap is loaded with dry ice.</t>
+  </si>
+  <si>
+    <t>Check that product line and argon line are closed. Release top valve on the receiver to make sure there is no extra pressure. Connect {equipment: peristaltic pump} to the bottom valve of the filter using {utensils: norprene hose}. Second end of the hose is securely fixed into receiving container {utensils: canister}, set the speed of peristaltic pump {setting}%. Start the pump. Continue the process until all ML is unloaded into respective receiver.</t>
+  </si>
+  <si>
+    <t>The filter cake is additionally dried on the filter using argon flow. Argon is set to {setting}l/min, check that outlet valve is opened and the stream is led to the ventilation. Argon line is opened. Drying on filter is continued for {setting} min. After required time is passed, the argon line is closed.</t>
+  </si>
+  <si>
+    <t>Membrane pump is set {setting}Torr.</t>
+  </si>
+  <si>
+    <t>Stop the pump. Connect {equipment: peristaltic pump} to the bottom valve of the filter using {utensils: norprene hose}. Second end of the hose is securely fixed into receiving container {utensils: canister}, set the speed of peristaltic pump {setting}%. Start the pump. Continue the process until all ML is unloaded into respective receiver.</t>
+  </si>
+  <si>
+    <t>The filter cake is additionally dried on the filter by keeping membrane pump sucking air through it. {equipment: membrane pump} is set to {setting}Torr. Drying on filter is continued for {setting} min. After required time is passed, the pump is stopped.</t>
   </si>
 </sst>
 </file>
@@ -180,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -188,11 +259,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,6 +393,46 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -541,248 +769,488 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D794DDE-2B33-47E5-885B-F9530E6FF737}">
-  <dimension ref="B4:G45"/>
+  <dimension ref="B4:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="3" max="3" width="21" style="5" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="91" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+    </row>
+    <row r="32" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="C33" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
+      <c r="C37" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="14"/>
+      <c r="C41" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C43" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+      <c r="C45" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+      <c r="C47" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+    </row>
+    <row r="49" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="10"/>
+      <c r="C49" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="10"/>
+      <c r="C53" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="14"/>
+      <c r="C55" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="16"/>
+      <c r="E55" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E10" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19"/>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20"/>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22"/>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-      <c r="C24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26"/>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30"/>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31"/>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32"/>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33"/>
-      <c r="C33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34"/>
-      <c r="C34" t="s">
+    <row r="56" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35"/>
-      <c r="C35" t="s">
+      <c r="D57" s="20"/>
+      <c r="E57" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37"/>
-      <c r="C37" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38"/>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39"/>
-      <c r="C39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40"/>
-      <c r="C40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41"/>
-      <c r="C41" t="s">
+      <c r="D59" s="20"/>
+      <c r="E59" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42"/>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:B27"/>
+    <mergeCell ref="B29:B41"/>
+    <mergeCell ref="B43:B55"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -806,7 +1274,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{18D659FD-1865-4C2D-A1DD-AAF003C58803}">
           <x14:formula1>
-            <xm:f>OFFSET(lists!$B$5, 0, 0, COUNTA(lists!$B$5:$B$45), 1)</xm:f>
+            <xm:f>OFFSET(lists!$B$5, 0, 0, COUNTA(lists!$B$5:$B$62), 1)</xm:f>
           </x14:formula1>
           <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>

</xml_diff>